<commit_message>
Commit Arquivo Cenários de Teste
</commit_message>
<xml_diff>
--- a/CenariosDeTesteBuildbox-KarenNunes.xlsx
+++ b/CenariosDeTesteBuildbox-KarenNunes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815" activeTab="1"/>
+    <workbookView windowWidth="19815" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Cenários de Testes" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>Cenários de Teste - Burger Eats</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Dispositivo</t>
   </si>
   <si>
-    <t>CENÁRIO DE TESTE 4 - Layout Responsivo</t>
+    <t>CENÁRIO DE TESTE 6 - Layout Responsivo</t>
   </si>
   <si>
     <t>CENÁRIO DE TESTE 1 - Cadastre-se para fazer entregas</t>
@@ -373,6 +373,9 @@
   <si>
     <t>2 - O sistema está permitindo o envio do CEP inválido e com o endereço diferente, e no campo "Bairro" aparece a mensagem: "undefined/undefined".
 - Passo a passo: Preencher um CEP válido e buscar o CEP. Preencher novamente com um CEP inválido e buscar o CEP.</t>
+  </si>
+  <si>
+    <t>CENÁRIO DE TESTE 4 - Layout Responsivo</t>
   </si>
   <si>
     <t>BUG IOS</t>
@@ -3591,8 +3594,8 @@
   <sheetPr/>
   <dimension ref="A1:AZ53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15.75"/>
@@ -4713,8 +4716,8 @@
   <sheetPr/>
   <dimension ref="A1:AZ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:B34"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -4849,16 +4852,16 @@
     </row>
     <row r="34" ht="15.75" spans="1:2">
       <c r="A34" s="15" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="B34" s="16"/>
     </row>
     <row r="35" ht="15" spans="1:2">
       <c r="A35" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2">

</xml_diff>